<commit_message>
try more features and different regressors
</commit_message>
<xml_diff>
--- a/Hyperparameter tuning log for Trips.xlsx
+++ b/Hyperparameter tuning log for Trips.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="0" windowWidth="25600" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
   <si>
     <t>Prep Notebook</t>
   </si>
@@ -172,6 +172,117 @@
   </si>
   <si>
     <t>Model getting better at predicting predominant case (on-time arrival). No late or extremely late observations predicted! Model seems unstable with many correlated features.</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V6</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V7</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V8</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V9</t>
+  </si>
+  <si>
+    <t>Make date attributes integers.</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V6 MODEL V8</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V7 MODEL V9</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V8 MODEL V10</t>
+  </si>
+  <si>
+    <t>sqrt mean sqr error minutes</t>
+  </si>
+  <si>
+    <t>median absolute error minutes</t>
+  </si>
+  <si>
+    <t>Still predicting predominent class (on-time). Using hourly and weekday features.</t>
+  </si>
+  <si>
+    <t>create one-hot encoded features for some date features.</t>
+  </si>
+  <si>
+    <t>Reduce one-hot date features.</t>
+  </si>
+  <si>
+    <t>All these features blew up the estimator.</t>
+  </si>
+  <si>
+    <t>Better but some dummy features are not integers. Buggy.</t>
+  </si>
+  <si>
+    <t>Misc one-hot features river gender, platform, metro, region.</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V9 MODEL V11</t>
+  </si>
+  <si>
+    <t>Ever so slightly better. Still bad.  Did use the region and metro dummies. On-time except for 12 observations. Still not beating random by much.</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V10</t>
+  </si>
+  <si>
+    <t>add previous ride in 1hr</t>
+  </si>
+  <si>
+    <t>Ever so slightly better.</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V10 MODEL V12</t>
+  </si>
+  <si>
+    <t>same</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V10 MODEL V13</t>
+  </si>
+  <si>
+    <t>Ridge</t>
+  </si>
+  <si>
+    <t>alpha = .75</t>
+  </si>
+  <si>
+    <t>Same. No improvement.</t>
+  </si>
+  <si>
+    <t>SGDRegressor</t>
+  </si>
+  <si>
+    <t>max_iter=10000</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V10 MODEL V14</t>
+  </si>
+  <si>
+    <t>Worse. But guessed 1/2 class 0 (on-time) and 1/2 3 (extremely late). Coefficients are huge. Conversion seems unstable for this highly dimensional data set. Even ID features had non-zero coefficients.</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V10 MODEL V15</t>
+  </si>
+  <si>
+    <t>try random forest regressor</t>
+  </si>
+  <si>
+    <t>try stochastic gradient descent regressor</t>
+  </si>
+  <si>
+    <t>RandomForestRegressor</t>
+  </si>
+  <si>
+    <t>max_depth=2, random_state=808, n_estimators=100</t>
+  </si>
+  <si>
+    <t>Found a whiff of signal. Not any better regression scores, roughly same. But classification scores improved from dreadful to just terrible. Most interesting: only used 8/214 features: 'scheduled_starts_at_pdt_hour',, 'scheduled_ends_at_pdt_hour', 'claimed_before_trip_start_secs', 'driver_previous_completed_trips', 'driver_signup_before_trip_start_secs', 'driver_signup_before_trip_claimed_secs', 'driver_created_at_pdt_dayofyear', 'driver_id'</t>
   </si>
 </sst>
 </file>
@@ -179,9 +290,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -213,16 +324,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -230,8 +354,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -275,8 +414,91 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -288,9 +510,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="43" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="43" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="126">
+    <cellStyle name="Calculation" xfId="43" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -312,6 +538,47 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -333,6 +600,47 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -662,10 +970,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="K1" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -678,19 +988,21 @@
     <col min="6" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" customWidth="1"/>
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="67.5" customWidth="1"/>
+    <col min="14" max="14" width="10.1640625" customWidth="1"/>
+    <col min="19" max="19" width="13.1640625" customWidth="1"/>
+    <col min="23" max="23" width="67.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" ht="45" customHeight="1">
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="45" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -731,31 +1043,37 @@
         <v>18</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="30">
+    <row r="4" spans="1:23" ht="30">
       <c r="A4" s="4">
         <v>43346</v>
       </c>
@@ -795,32 +1113,40 @@
       <c r="M4">
         <v>0.32400000000000001</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="7">
+        <f>SQRT(O4)/60</f>
+        <v>311.88457845455866</v>
+      </c>
+      <c r="O4">
         <v>350179165</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>0.32400000000000001</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>3015</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>1855</v>
       </c>
-      <c r="R4">
+      <c r="S4" s="8">
+        <f>R4/60</f>
+        <v>30.916666666666668</v>
+      </c>
+      <c r="T4">
         <v>0.72</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>0.48</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>0.56999999999999995</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="30">
+    <row r="5" spans="1:23" ht="30">
       <c r="A5" s="4">
         <v>43358</v>
       </c>
@@ -860,32 +1186,40 @@
       <c r="M5">
         <v>-67.956000000000003</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="7">
+        <f t="shared" ref="N5:N10" si="0">SQRT(O5)/60</f>
+        <v>199.78374767065847</v>
+      </c>
+      <c r="O5">
         <v>143688765</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>-67.959999999999994</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>3405</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>2119</v>
       </c>
-      <c r="R5">
+      <c r="S5" s="8">
+        <f>R5/60</f>
+        <v>35.31666666666667</v>
+      </c>
+      <c r="T5">
         <v>0.72</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>0.48</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>0.56999999999999995</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="30">
+    <row r="6" spans="1:23" ht="30">
       <c r="A6" s="4">
         <v>43359</v>
       </c>
@@ -925,32 +1259,40 @@
       <c r="M6">
         <v>-67.956000000000003</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="7">
+        <f t="shared" si="0"/>
+        <v>199.78374767065847</v>
+      </c>
+      <c r="O6">
         <v>143688765</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>-67.959999999999994</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>3405</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>2119</v>
       </c>
-      <c r="R6">
+      <c r="S6" s="8">
+        <f>R6/60</f>
+        <v>35.31666666666667</v>
+      </c>
+      <c r="T6">
         <v>0.72</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>0.48</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>0.56999999999999995</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="30">
+    <row r="7" spans="1:23" ht="30">
       <c r="A7" s="4">
         <v>43359</v>
       </c>
@@ -987,32 +1329,40 @@
       <c r="M7">
         <v>-67.984999999999999</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="7">
+        <f t="shared" si="0"/>
+        <v>199.82553154078076</v>
+      </c>
+      <c r="O7">
         <v>143748875</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>-67.989000000000004</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>3413</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>2122</v>
       </c>
-      <c r="R7">
+      <c r="S7" s="8">
+        <f>R7/60</f>
+        <v>35.366666666666667</v>
+      </c>
+      <c r="T7">
         <v>0.72</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>0.48</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>0.56999999999999995</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="45">
+    <row r="8" spans="1:23" ht="45">
       <c r="A8" s="4">
         <v>43359</v>
       </c>
@@ -1049,32 +1399,40 @@
       <c r="M8">
         <v>-2.3E-2</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="7">
+        <f t="shared" si="0"/>
+        <v>24.33530813904402</v>
+      </c>
+      <c r="O8">
         <v>2131946</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>-2.3E-2</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>447</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>332</v>
       </c>
-      <c r="R8">
+      <c r="S8" s="8">
+        <f>R8/60</f>
+        <v>5.5333333333333332</v>
+      </c>
+      <c r="T8">
         <v>0.73</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>0.83</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>0.77</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="30">
+    <row r="9" spans="1:23" ht="30">
       <c r="A9" s="4">
         <v>43359</v>
       </c>
@@ -1111,32 +1469,40 @@
       <c r="M9">
         <v>-2.7E-2</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="7">
+        <f t="shared" si="0"/>
+        <v>24.386027420089015</v>
+      </c>
+      <c r="O9">
         <v>2140842</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>-2.7E-2</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>455</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>335</v>
       </c>
-      <c r="R9">
+      <c r="S9" s="8">
+        <f>R9/60</f>
+        <v>5.583333333333333</v>
+      </c>
+      <c r="T9">
         <v>0.73</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>0.82</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>0.77</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="45">
+    <row r="10" spans="1:23" ht="45">
       <c r="A10" s="4">
         <v>43359</v>
       </c>
@@ -1173,29 +1539,587 @@
       <c r="M10">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="7">
+        <f t="shared" si="0"/>
+        <v>8.3417790535219627</v>
+      </c>
+      <c r="O10">
         <v>250507</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>375</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>286</v>
       </c>
-      <c r="R10">
+      <c r="S10" s="8">
+        <f>R10/60</f>
+        <v>4.7666666666666666</v>
+      </c>
+      <c r="T10">
         <v>0.74</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>0.84</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>0.77</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="45">
+      <c r="A11" s="4">
+        <v>43366</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11">
+        <v>125675</v>
+      </c>
+      <c r="E11">
+        <v>361</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11">
+        <v>100540</v>
+      </c>
+      <c r="K11">
+        <v>25135</v>
+      </c>
+      <c r="L11" s="5">
+        <v>1.07966610303269E-3</v>
+      </c>
+      <c r="M11">
+        <v>-7.0243232983993599E+22</v>
+      </c>
+      <c r="N11">
+        <v>2262893661113.6499</v>
+      </c>
+      <c r="O11">
+        <v>1.84344757974299E+28</v>
+      </c>
+      <c r="P11">
+        <v>-7.0246027733455797E+22</v>
+      </c>
+      <c r="Q11">
+        <v>856398605935</v>
+      </c>
+      <c r="R11">
+        <v>281</v>
+      </c>
+      <c r="S11" s="6">
+        <v>4.68</v>
+      </c>
+      <c r="T11">
+        <v>0.72</v>
+      </c>
+      <c r="U11">
+        <v>0.84</v>
+      </c>
+      <c r="V11">
+        <v>0.77</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="30">
+      <c r="A12" s="4">
+        <v>43366</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12">
+        <v>125675</v>
+      </c>
+      <c r="E12">
+        <v>215</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12">
+        <v>100540</v>
+      </c>
+      <c r="K12">
+        <v>25135</v>
+      </c>
+      <c r="L12" s="5">
+        <v>-1.268815451684E-2</v>
+      </c>
+      <c r="M12">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="N12">
+        <v>8.33</v>
+      </c>
+      <c r="O12">
+        <v>249937</v>
+      </c>
+      <c r="P12">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="Q12">
+        <v>374</v>
+      </c>
+      <c r="R12">
+        <v>285</v>
+      </c>
+      <c r="S12">
+        <v>4.75</v>
+      </c>
+      <c r="T12">
+        <v>0.71</v>
+      </c>
+      <c r="U12">
+        <v>0.84</v>
+      </c>
+      <c r="V12">
+        <v>0.77</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="30">
+      <c r="A13" s="4">
+        <v>43366</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>125675</v>
+      </c>
+      <c r="E13">
+        <v>172</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13">
+        <v>100540</v>
+      </c>
+      <c r="K13">
+        <v>25135</v>
+      </c>
+      <c r="L13" s="5">
+        <v>-1.33755032934903E-2</v>
+      </c>
+      <c r="M13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="N13">
+        <v>8.33</v>
+      </c>
+      <c r="O13">
+        <v>250014</v>
+      </c>
+      <c r="P13">
+        <v>4.7E-2</v>
+      </c>
+      <c r="Q13">
+        <v>375</v>
+      </c>
+      <c r="R13">
+        <v>286</v>
+      </c>
+      <c r="S13">
+        <v>4.76</v>
+      </c>
+      <c r="T13">
+        <v>0.73</v>
+      </c>
+      <c r="U13">
+        <v>0.84</v>
+      </c>
+      <c r="V13">
+        <v>0.77</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="45">
+      <c r="A14" s="4">
+        <v>43366</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14">
+        <v>125675</v>
+      </c>
+      <c r="E14">
+        <v>213</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14">
+        <v>100540</v>
+      </c>
+      <c r="K14">
+        <v>25135</v>
+      </c>
+      <c r="L14" s="5">
+        <v>-7.0833111987587899E-3</v>
+      </c>
+      <c r="M14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="N14">
+        <v>8.32</v>
+      </c>
+      <c r="O14">
+        <v>248996</v>
+      </c>
+      <c r="P14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="Q14">
+        <v>373</v>
+      </c>
+      <c r="R14">
+        <v>284</v>
+      </c>
+      <c r="S14">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="T14">
+        <v>0.73</v>
+      </c>
+      <c r="U14">
+        <v>0.84</v>
+      </c>
+      <c r="V14">
+        <v>0.77</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15" s="4">
+        <v>43373</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15">
+        <v>125675</v>
+      </c>
+      <c r="E15">
+        <v>214</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15">
+        <v>100540</v>
+      </c>
+      <c r="K15">
+        <v>25135</v>
+      </c>
+      <c r="L15" s="5">
+        <v>-8.1993510577104793E-3</v>
+      </c>
+      <c r="M15">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="N15">
+        <v>8.31</v>
+      </c>
+      <c r="O15">
+        <v>248860</v>
+      </c>
+      <c r="P15">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="Q15">
+        <v>373</v>
+      </c>
+      <c r="R15">
+        <v>284</v>
+      </c>
+      <c r="S15">
+        <v>4.72</v>
+      </c>
+      <c r="T15">
+        <v>0.72</v>
+      </c>
+      <c r="U15">
+        <v>0.84</v>
+      </c>
+      <c r="V15">
+        <v>0.77</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16" s="4">
+        <v>43373</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16">
+        <v>125675</v>
+      </c>
+      <c r="E16">
+        <v>214</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16">
+        <v>100540</v>
+      </c>
+      <c r="K16">
+        <v>25135</v>
+      </c>
+      <c r="L16" s="5">
+        <v>-6.9221370261790798E-3</v>
+      </c>
+      <c r="M16">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="N16">
+        <v>8.31</v>
+      </c>
+      <c r="O16">
+        <v>248752</v>
+      </c>
+      <c r="P16">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="Q16">
+        <v>373</v>
+      </c>
+      <c r="R16">
+        <v>284</v>
+      </c>
+      <c r="S16">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="T16">
+        <v>0.73</v>
+      </c>
+      <c r="U16">
+        <v>0.84</v>
+      </c>
+      <c r="V16">
+        <v>0.77</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="45">
+      <c r="A17" s="4">
+        <v>43373</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17">
+        <v>125675</v>
+      </c>
+      <c r="E17">
+        <v>214</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17">
+        <v>100540</v>
+      </c>
+      <c r="K17">
+        <v>25135</v>
+      </c>
+      <c r="L17" s="5">
+        <v>-1.36977094646201E-2</v>
+      </c>
+      <c r="M17">
+        <v>-4.3770976965667699E+40</v>
+      </c>
+      <c r="N17">
+        <v>1.7968854311876E+21</v>
+      </c>
+      <c r="O17">
+        <v>1.1623670110131301E+46</v>
+      </c>
+      <c r="P17">
+        <v>-4.4292914097110604E+40</v>
+      </c>
+      <c r="Q17">
+        <v>8.0596155433541196E+22</v>
+      </c>
+      <c r="R17">
+        <v>5.9380573630645297E+22</v>
+      </c>
+      <c r="S17">
+        <v>9.89676227177422E+20</v>
+      </c>
+      <c r="T17">
+        <v>0.71</v>
+      </c>
+      <c r="U17">
+        <v>0.43</v>
+      </c>
+      <c r="V17">
+        <v>0.53</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="105">
+      <c r="A18" s="4">
+        <v>43377</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18">
+        <v>125675</v>
+      </c>
+      <c r="E18">
+        <v>214</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18">
+        <v>100540</v>
+      </c>
+      <c r="K18">
+        <v>25135</v>
+      </c>
+      <c r="L18" s="5">
+        <v>-3.2080185331021201E-2</v>
+      </c>
+      <c r="M18">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="N18">
+        <v>8.36</v>
+      </c>
+      <c r="O18">
+        <v>251546</v>
+      </c>
+      <c r="P18">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="Q18">
+        <v>376</v>
+      </c>
+      <c r="R18">
+        <v>286</v>
+      </c>
+      <c r="S18">
+        <v>4.76</v>
+      </c>
+      <c r="T18">
+        <v>0.75</v>
+      </c>
+      <c r="U18">
+        <v>0.84</v>
+      </c>
+      <c r="V18">
+        <v>0.77</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test for leakage, lateness to location feature
</commit_message>
<xml_diff>
--- a/Hyperparameter tuning log for Trips.xlsx
+++ b/Hyperparameter tuning log for Trips.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="114">
   <si>
     <t>Prep Notebook</t>
   </si>
@@ -336,7 +336,31 @@
     <t>max_depth=4, random_state=808, n_estimators=201</t>
   </si>
   <si>
-    <t>all scores imporved. medabserror down 17 seconds to 3min42sec. Explaining 26% of the variance up from 20%. New feature was #1 kicking driver_id down to #7. Top 10 features used: ['avg_prior_arrived_late_seconds', 'claimed_before_trip_start_secs', 'origin_location_id', 'driver_previous_completed_trips', 'driver_home_lon', 'driver_home_lat', 'driver_id', 'scheduled_starts_at_pdt_hour', 'driver_created_at_pdt_dayofyear', 'destination_location_id']  Note that 28 features were above 1% importance, indicating a long tail of causes. Now 5 of top 10 are about driver (independent of the trip) and 5 are about trip. Precision of the late classes in 40-50% range!</t>
+    <t>Trips lab notebook Will driver be late? PREP V11 MODEL V20</t>
+  </si>
+  <si>
+    <t>test for leakage train on older data and test on newer data</t>
+  </si>
+  <si>
+    <t>all scores improved. medabserror down 17 seconds to 3min42sec. Explaining 26% of the variance up from 20%. New feature was #1 kicking driver_id down to #7. Top 10 features used: ['avg_prior_arrived_late_seconds', 'claimed_before_trip_start_secs', 'origin_location_id', 'driver_previous_completed_trips', 'driver_home_lon', 'driver_home_lat', 'driver_id', 'scheduled_starts_at_pdt_hour', 'driver_created_at_pdt_dayofyear', 'destination_location_id']  Note that 28 features were above 1% importance, indicating a long tail of causes. Now 5 of top 10 are about driver (independent of the trip) and 5 are about trip. Precision of the late classes in 40-50% range!</t>
+  </si>
+  <si>
+    <t>Model did not perform as well on this test set over a seprate, later time frame. Explaining 19% of variance compared to 26% in random test set. Precision of late classes in 20%-30% range. Leakage existed in some way in randomly selected test set. Possibly due to different drivers driving in different times of the year. Top 10 features used: ['avg_prior_arrived_late_seconds', 'claimed_before_trip_start_secs', 'driver_previous_completed_trips', 'driver_home_lon', 'driver_id', 'driver_home_lat', 'origin_location_id', 'scheduled_starts_at_pdt_hour', 'driver_created_at_pdt_dayofyear', 'origin_lon']. Similar importance features.</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V12</t>
+  </si>
+  <si>
+    <t>added feature avg_prior_arrived_late_seconds_to_origin_location</t>
+  </si>
+  <si>
+    <t>Trips lab notebook Will driver be late? PREP V12 MODEL V21</t>
+  </si>
+  <si>
+    <t>continute to use time series test set and test new feature</t>
+  </si>
+  <si>
+    <t>Model performance improved not back up to level with randomly selected test set. Explained 19% of variance. New feature was used #6 rank importance. Interesting that origin_location which was #3 now #8 and driver_id is #3, up from #5. This indicates there are still driver and location patterns unrelated to past performance of target variable (lateness). Precision of late classes in high 20%s. The average precision/recall/F1 are dominated by the large early arrival class. Top 10 features used: ['avg_prior_arrived_late_seconds', 'claimed_before_trip_start_secs', 'driver_id', 'driver_previous_completed_trips', 'driver_home_lat', 'avg_prior_arrived_late_seconds_to_origin_location', 'driver_home_lon', 'origin_location_id', 'scheduled_starts_at_pdt_hour', 'destination_location_id']</t>
   </si>
 </sst>
 </file>
@@ -424,7 +448,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="154">
+  <cellStyleXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -469,6 +493,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -597,7 +637,7 @@
     <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="43" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="43" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="154">
+  <cellStyles count="170">
     <cellStyle name="Calculation" xfId="43" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -675,6 +715,14 @@
     <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -751,6 +799,14 @@
     <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1080,12 +1136,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="X23" sqref="X23"/>
+      <selection pane="bottomLeft" activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2531,7 +2587,155 @@
         <v>157</v>
       </c>
       <c r="X22" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="135">
+      <c r="A23" s="4">
+        <v>43415</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23">
+        <v>125675</v>
+      </c>
+      <c r="E23">
+        <v>215</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>105</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H23" t="s">
+        <v>99</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23">
+        <v>100198</v>
+      </c>
+      <c r="K23">
+        <v>25477</v>
+      </c>
+      <c r="L23" s="5">
+        <v>-8.6116083461327993E-3</v>
+      </c>
+      <c r="M23">
+        <v>0.18</v>
+      </c>
+      <c r="N23">
+        <v>7.57</v>
+      </c>
+      <c r="O23">
+        <v>206403</v>
+      </c>
+      <c r="P23">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="Q23">
+        <v>337</v>
+      </c>
+      <c r="R23">
+        <v>251</v>
+      </c>
+      <c r="S23">
+        <v>4.18</v>
+      </c>
+      <c r="T23">
+        <v>0.75</v>
+      </c>
+      <c r="U23">
+        <v>0.83</v>
+      </c>
+      <c r="V23">
+        <v>0.77</v>
+      </c>
+      <c r="W23">
+        <v>152</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="165">
+      <c r="A24" s="4">
+        <v>43415</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24">
+        <v>125675</v>
+      </c>
+      <c r="E24">
+        <v>216</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H24" t="s">
+        <v>99</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J24">
+        <v>100198</v>
+      </c>
+      <c r="K24">
+        <v>25477</v>
+      </c>
+      <c r="L24" s="5">
+        <v>-8.3118441055710195E-3</v>
+      </c>
+      <c r="M24">
+        <v>0.186</v>
+      </c>
+      <c r="N24">
+        <v>7.54</v>
+      </c>
+      <c r="O24">
+        <v>204536</v>
+      </c>
+      <c r="P24">
+        <v>0.186</v>
+      </c>
+      <c r="Q24">
+        <v>334</v>
+      </c>
+      <c r="R24">
+        <v>245</v>
+      </c>
+      <c r="S24">
+        <v>4.09</v>
+      </c>
+      <c r="T24">
+        <v>0.75</v>
+      </c>
+      <c r="U24">
+        <v>0.83</v>
+      </c>
+      <c r="V24">
+        <v>0.77</v>
+      </c>
+      <c r="W24">
+        <v>145</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>